<commit_message>
fixed export and fixing maps
</commit_message>
<xml_diff>
--- a/municipal/ENG/Main Information/Municipality area/Abasha Municipality.xlsx
+++ b/municipal/ENG/Main Information/Municipality area/Abasha Municipality.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\დემოგრაფია\Tamunas cxrilebi\inglisuri\cx 29 - eng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tgrigolishvili\Desktop\ფართობი ქარ. EN\Municipality area\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CF419A-81EA-4B65-B0F3-12C26BB38D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="585" yWindow="180" windowWidth="12345" windowHeight="7905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="585" yWindow="180" windowWidth="12345" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -25,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Area</t>
   </si>
   <si>
     <t>(sq. km)</t>
-  </si>
-  <si>
-    <t>(according to the population census data)</t>
   </si>
   <si>
     <t>Area of the municipality of Abasha</t>
@@ -42,11 +38,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,12 +81,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -106,7 +96,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -128,30 +118,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -168,17 +134,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -207,45 +162,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -254,8 +190,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal_Mosaxleoba na 1.1 raionebis mixedvit" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal_Mosaxleoba na 1.1 raionebis mixedvit" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -532,62 +468,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="16" customWidth="1"/>
-    <col min="2" max="4" width="8.7109375" style="15" customWidth="1"/>
-    <col min="5" max="18" width="5.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9.140625" style="15"/>
+    <col min="1" max="1" width="15.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="8" customWidth="1"/>
+    <col min="3" max="16" width="5.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:2" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="12"/>
     </row>
-    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="12"/>
-    </row>
-    <row r="4" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+    <row r="2" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="1">
-        <v>1989</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2002</v>
-      </c>
-      <c r="D5" s="3">
+    <row r="4" spans="1:2" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="1">
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+    <row r="5" spans="1:2" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="4">
-        <v>320.5</v>
-      </c>
-      <c r="C6" s="5">
-        <v>322.5</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="B5" s="2">
         <v>322.5</v>
       </c>
     </row>

</xml_diff>